<commit_message>
End of 2024 Update
</commit_message>
<xml_diff>
--- a/GameDefinitions/YsViCharactersListWithIds.xlsx
+++ b/GameDefinitions/YsViCharactersListWithIds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://raidermailwright-my.sharepoint.com/personal/rynders_3_wright_edu/Documents/Documents/YsViReverseEngineering/YsViDecomp/GameDefinitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{A29B733F-1F98-42D4-8048-96294F52CE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D898E02A-6E85-4882-B096-4B8A145A0731}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="8_{A29B733F-1F98-42D4-8048-96294F52CE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{298F655D-DD3A-413F-95CE-79E5C9DC9B32}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E20CABA4-0534-4FA0-B082-09042A593522}"/>
   </bookViews>
@@ -287,9 +287,6 @@
     <t>0x69</t>
   </si>
   <si>
-    <t>Zakuson</t>
-  </si>
-  <si>
     <t>0x67</t>
   </si>
   <si>
@@ -579,6 +576,9 @@
   </si>
   <si>
     <t>0x65</t>
+  </si>
+  <si>
+    <t>Zakuson/String</t>
   </si>
 </sst>
 </file>
@@ -631,10 +631,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -956,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600D4736-27BD-4DA0-AF1F-0BD704FAFCD8}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,13 +984,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2">
         <v>101</v>
@@ -1025,10 +1021,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1056,109 +1052,109 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6">
         <v>121</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7">
         <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9">
         <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10">
         <v>112</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11">
         <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D12">
         <v>97</v>
@@ -1172,7 +1168,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D13">
         <v>92</v>
@@ -1203,7 +1199,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D15">
         <v>72</v>
@@ -1214,16 +1210,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1251,24 +1247,24 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D18">
         <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D19">
         <v>142</v>
@@ -1285,13 +1281,13 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20">
         <v>109</v>
       </c>
       <c r="E20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1302,7 +1298,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D21">
         <v>90</v>
@@ -1313,13 +1309,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D22">
         <v>138</v>
@@ -1336,7 +1332,7 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D23">
         <v>77</v>
@@ -1353,30 +1349,30 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24">
         <v>108</v>
       </c>
       <c r="E24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D25">
         <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1387,30 +1383,30 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26">
         <v>135</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1435,7 +1431,7 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29">
         <v>102</v>
@@ -1449,30 +1445,30 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D30">
         <v>128</v>
       </c>
       <c r="E30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D31">
         <v>125</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1483,13 +1479,13 @@
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32">
         <v>104</v>
       </c>
       <c r="E32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1500,30 +1496,30 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D33">
         <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D34">
         <v>141</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1534,61 +1530,61 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D35">
         <v>123</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D36">
         <v>130</v>
       </c>
       <c r="E36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D38">
         <v>143</v>
       </c>
       <c r="E38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1599,7 +1595,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D39">
         <v>134</v>
@@ -1616,30 +1612,30 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D40">
         <v>88</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D41">
         <v>91</v>
       </c>
       <c r="E41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1650,13 +1646,13 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D42">
         <v>122</v>
       </c>
       <c r="E42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1667,7 +1663,7 @@
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43">
         <v>100</v>
@@ -1678,19 +1674,19 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" t="s">
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D44">
         <v>124</v>
       </c>
       <c r="E44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1707,7 +1703,7 @@
         <v>74</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1735,13 +1731,13 @@
         <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D47">
         <v>132</v>
       </c>
       <c r="E47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1752,13 +1748,13 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D48">
         <v>126</v>
       </c>
       <c r="E48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1769,7 +1765,7 @@
         <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D49">
         <v>76</v>
@@ -1803,13 +1799,13 @@
         <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D51">
         <v>136</v>
       </c>
       <c r="E51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1820,13 +1816,13 @@
         <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D52">
         <v>133</v>
       </c>
       <c r="E52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1854,13 +1850,13 @@
         <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D54">
         <v>83</v>
       </c>
       <c r="E54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,7 +1884,7 @@
         <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D56">
         <v>111</v>
@@ -1905,13 +1901,13 @@
         <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D57">
         <v>129</v>
       </c>
       <c r="E57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1922,30 +1918,30 @@
         <v>58</v>
       </c>
       <c r="C58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D58">
         <v>86</v>
       </c>
       <c r="E58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B59" t="s">
         <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D59">
         <v>127</v>
       </c>
       <c r="E59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1956,13 +1952,13 @@
         <v>60</v>
       </c>
       <c r="C60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D60">
         <v>103</v>
       </c>
       <c r="E60" t="s">
-        <v>83</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1973,7 +1969,7 @@
         <v>61</v>
       </c>
       <c r="C61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D61">
         <v>78</v>

</xml_diff>